<commit_message>
Update segment region mapping
</commit_message>
<xml_diff>
--- a/data/Mapping_countries_to_fund_regions.xlsx
+++ b/data/Mapping_countries_to_fund_regions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisarennels/JuliaProjects/RFF Model/RffModel.jl/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisarennels/.julia/dev/MimiGIVE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328C94E5-06CC-E64A-BF97-CC5A300027EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33807080-C627-DD4D-AD6A-BA4ABF491CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14740" yWindow="460" windowWidth="26200" windowHeight="22540" activeTab="3" xr2:uid="{DC6EAC6E-16BD-8449-AB04-434FF248409A}"/>
+    <workbookView xWindow="44500" yWindow="960" windowWidth="26200" windowHeight="21100" activeTab="3" xr2:uid="{DC6EAC6E-16BD-8449-AB04-434FF248409A}"/>
   </bookViews>
   <sheets>
     <sheet name="FUND" sheetId="2" r:id="rId1"/>
@@ -21,17 +21,27 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FUND!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="766">
   <si>
     <t>USA</t>
   </si>
@@ -8010,7 +8020,7 @@
       <c r="I257" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D257">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D257">
     <sortCondition ref="A2:A257"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12428,10 +12438,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BD5947-2972-7A4B-B98A-AA4D8BBB6678}">
-  <dimension ref="A1:C142"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="E157" sqref="E157"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12661,59 +12671,59 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>226</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP(A18,FUND!A:C, 3, FALSE)</f>
-        <v>CAN</v>
+        <v>SEA</v>
       </c>
       <c r="C18" t="str">
         <f>VLOOKUP(A18,FUND!A:D, 4, FALSE)</f>
-        <v>Canada</v>
+        <v>Brunei</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>232</v>
+        <v>2</v>
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP(A19,FUND!A:C, 3, FALSE)</f>
-        <v>LAM</v>
+        <v>CAN</v>
       </c>
       <c r="C19" t="str">
         <f>VLOOKUP(A19,FUND!A:D, 4, FALSE)</f>
-        <v>Chile</v>
+        <v>Canada</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP(A20,FUND!A:C, 3, FALSE)</f>
-        <v>CHI</v>
+        <v>LAM</v>
       </c>
       <c r="C20" t="str">
         <f>VLOOKUP(A20,FUND!A:D, 4, FALSE)</f>
-        <v>China</v>
+        <v>Chile</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP(A21,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>CHI</v>
       </c>
       <c r="C21" t="str">
         <f>VLOOKUP(A21,FUND!A:D, 4, FALSE)</f>
-        <v>Côte d'Ivoire</v>
+        <v>China</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(A22,FUND!A:C, 3, FALSE)</f>
@@ -12721,12 +12731,12 @@
       </c>
       <c r="C22" t="str">
         <f>VLOOKUP(A22,FUND!A:D, 4, FALSE)</f>
-        <v>Cameroon</v>
+        <v>Côte d'Ivoire</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP(A23,FUND!A:C, 3, FALSE)</f>
@@ -12734,12 +12744,12 @@
       </c>
       <c r="C23" t="str">
         <f>VLOOKUP(A23,FUND!A:D, 4, FALSE)</f>
-        <v>Congo, the Democratic Republic of the</v>
+        <v>Cameroon</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B24" t="str">
         <f>VLOOKUP(A24,FUND!A:C, 3, FALSE)</f>
@@ -12747,90 +12757,90 @@
       </c>
       <c r="C24" t="str">
         <f>VLOOKUP(A24,FUND!A:D, 4, FALSE)</f>
-        <v>Congo</v>
+        <v>Congo, the Democratic Republic of the</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B25" t="str">
         <f>VLOOKUP(A25,FUND!A:C, 3, FALSE)</f>
-        <v>LAM</v>
+        <v>SSA</v>
       </c>
       <c r="C25" t="str">
         <f>VLOOKUP(A25,FUND!A:D, 4, FALSE)</f>
-        <v>Colombia</v>
+        <v>Congo</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B26" t="str">
         <f>VLOOKUP(A26,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>LAM</v>
       </c>
       <c r="C26" t="str">
         <f>VLOOKUP(A26,FUND!A:D, 4, FALSE)</f>
-        <v>Comoros</v>
+        <v>Colombia</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B27" t="str">
         <f>VLOOKUP(A27,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>SIS</v>
       </c>
       <c r="C27" t="str">
         <f>VLOOKUP(A27,FUND!A:D, 4, FALSE)</f>
-        <v>Cape Verde</v>
+        <v>Comoros</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B28" t="str">
         <f>VLOOKUP(A28,FUND!A:C, 3, FALSE)</f>
-        <v>CAM</v>
+        <v>SSA</v>
       </c>
       <c r="C28" t="str">
         <f>VLOOKUP(A28,FUND!A:D, 4, FALSE)</f>
-        <v>Costa Rica</v>
+        <v>Cape Verde</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B29" t="str">
         <f>VLOOKUP(A29,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>CAM</v>
       </c>
       <c r="C29" t="str">
         <f>VLOOKUP(A29,FUND!A:D, 4, FALSE)</f>
-        <v>Cuba</v>
+        <v>Costa Rica</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B30" t="str">
         <f>VLOOKUP(A30,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SIS</v>
       </c>
       <c r="C30" t="str">
         <f>VLOOKUP(A30,FUND!A:D, 4, FALSE)</f>
-        <v>Cyprus</v>
+        <v>Cuba</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B31" t="str">
         <f>VLOOKUP(A31,FUND!A:C, 3, FALSE)</f>
@@ -12838,220 +12848,220 @@
       </c>
       <c r="C31" t="str">
         <f>VLOOKUP(A31,FUND!A:D, 4, FALSE)</f>
-        <v>Germany</v>
+        <v>Cyprus</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B32" t="str">
         <f>VLOOKUP(A32,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>WEU</v>
       </c>
       <c r="C32" t="str">
         <f>VLOOKUP(A32,FUND!A:D, 4, FALSE)</f>
-        <v>Djibouti</v>
+        <v>Germany</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B33" t="str">
         <f>VLOOKUP(A33,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SSA</v>
       </c>
       <c r="C33" t="str">
         <f>VLOOKUP(A33,FUND!A:D, 4, FALSE)</f>
-        <v>Denmark</v>
+        <v>Djibouti</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B34" t="str">
         <f>VLOOKUP(A34,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>WEU</v>
       </c>
       <c r="C34" t="str">
         <f>VLOOKUP(A34,FUND!A:D, 4, FALSE)</f>
-        <v>Dominican Republic</v>
+        <v>Denmark</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B35" t="str">
         <f>VLOOKUP(A35,FUND!A:C, 3, FALSE)</f>
-        <v>MAF</v>
+        <v>SIS</v>
       </c>
       <c r="C35" t="str">
         <f>VLOOKUP(A35,FUND!A:D, 4, FALSE)</f>
-        <v>Algeria</v>
+        <v>Dominican Republic</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B36" t="str">
         <f>VLOOKUP(A36,FUND!A:C, 3, FALSE)</f>
-        <v>LAM</v>
+        <v>MAF</v>
       </c>
       <c r="C36" t="str">
         <f>VLOOKUP(A36,FUND!A:D, 4, FALSE)</f>
-        <v>Ecuador</v>
+        <v>Algeria</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B37" t="str">
         <f>VLOOKUP(A37,FUND!A:C, 3, FALSE)</f>
-        <v>MAF</v>
+        <v>LAM</v>
       </c>
       <c r="C37" t="str">
         <f>VLOOKUP(A37,FUND!A:D, 4, FALSE)</f>
-        <v>Egypt</v>
+        <v>Ecuador</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B38" t="str">
         <f>VLOOKUP(A38,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>MAF</v>
       </c>
       <c r="C38" t="str">
         <f>VLOOKUP(A38,FUND!A:D, 4, FALSE)</f>
-        <v>Eritrea</v>
+        <v>Egypt</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B39" t="str">
         <f>VLOOKUP(A39,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SSA</v>
       </c>
       <c r="C39" t="str">
         <f>VLOOKUP(A39,FUND!A:D, 4, FALSE)</f>
-        <v>Spain</v>
+        <v>Eritrea</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B40" t="str">
         <f>VLOOKUP(A40,FUND!A:C, 3, FALSE)</f>
-        <v>FSU</v>
+        <v>WEU</v>
       </c>
       <c r="C40" t="str">
         <f>VLOOKUP(A40,FUND!A:D, 4, FALSE)</f>
-        <v>Estonia</v>
+        <v>Spain</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B41" t="str">
         <f>VLOOKUP(A41,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>FSU</v>
       </c>
       <c r="C41" t="str">
         <f>VLOOKUP(A41,FUND!A:D, 4, FALSE)</f>
-        <v>Finland</v>
+        <v>Estonia</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B42" t="str">
         <f>VLOOKUP(A42,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>WEU</v>
       </c>
       <c r="C42" t="str">
         <f>VLOOKUP(A42,FUND!A:D, 4, FALSE)</f>
-        <v>Fiji</v>
+        <v>Finland</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B43" t="str">
         <f>VLOOKUP(A43,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SIS</v>
       </c>
       <c r="C43" t="str">
         <f>VLOOKUP(A43,FUND!A:D, 4, FALSE)</f>
-        <v>France</v>
+        <v>Fiji</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B44" t="str">
         <f>VLOOKUP(A44,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>WEU</v>
       </c>
       <c r="C44" t="str">
         <f>VLOOKUP(A44,FUND!A:D, 4, FALSE)</f>
-        <v>Gabon</v>
+        <v>France</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B45" t="str">
         <f>VLOOKUP(A45,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SSA</v>
       </c>
       <c r="C45" t="str">
         <f>VLOOKUP(A45,FUND!A:D, 4, FALSE)</f>
-        <v>United Kingdom</v>
+        <v>Gabon</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B46" t="str">
         <f>VLOOKUP(A46,FUND!A:C, 3, FALSE)</f>
-        <v>FSU</v>
+        <v>WEU</v>
       </c>
       <c r="C46" t="str">
         <f>VLOOKUP(A46,FUND!A:D, 4, FALSE)</f>
-        <v>Georgia</v>
+        <v>United Kingdom</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B47" t="str">
         <f>VLOOKUP(A47,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>FSU</v>
       </c>
       <c r="C47" t="str">
         <f>VLOOKUP(A47,FUND!A:D, 4, FALSE)</f>
-        <v>Ghana</v>
+        <v>Georgia</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B48" t="str">
         <f>VLOOKUP(A48,FUND!A:C, 3, FALSE)</f>
@@ -13059,12 +13069,12 @@
       </c>
       <c r="C48" t="str">
         <f>VLOOKUP(A48,FUND!A:D, 4, FALSE)</f>
-        <v>Guinea</v>
+        <v>Ghana</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B49" t="str">
         <f>VLOOKUP(A49,FUND!A:C, 3, FALSE)</f>
@@ -13072,12 +13082,12 @@
       </c>
       <c r="C49" t="str">
         <f>VLOOKUP(A49,FUND!A:D, 4, FALSE)</f>
-        <v>Gambia</v>
+        <v>Guinea</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B50" t="str">
         <f>VLOOKUP(A50,FUND!A:C, 3, FALSE)</f>
@@ -13085,12 +13095,12 @@
       </c>
       <c r="C50" t="str">
         <f>VLOOKUP(A50,FUND!A:D, 4, FALSE)</f>
-        <v>Guinea-Bissau</v>
+        <v>Gambia</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B51" t="str">
         <f>VLOOKUP(A51,FUND!A:C, 3, FALSE)</f>
@@ -13098,168 +13108,168 @@
       </c>
       <c r="C51" t="str">
         <f>VLOOKUP(A51,FUND!A:D, 4, FALSE)</f>
-        <v>Equatorial Guinea</v>
+        <v>Guinea-Bissau</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B52" t="str">
         <f>VLOOKUP(A52,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SSA</v>
       </c>
       <c r="C52" t="str">
         <f>VLOOKUP(A52,FUND!A:D, 4, FALSE)</f>
-        <v>Greece</v>
+        <v>Equatorial Guinea</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B53" t="str">
         <f>VLOOKUP(A53,FUND!A:C, 3, FALSE)</f>
-        <v>CAM</v>
+        <v>WEU</v>
       </c>
       <c r="C53" t="str">
         <f>VLOOKUP(A53,FUND!A:D, 4, FALSE)</f>
-        <v>Guatemala</v>
+        <v>Greece</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B54" t="str">
         <f>VLOOKUP(A54,FUND!A:C, 3, FALSE)</f>
-        <v>LAM</v>
+        <v>CAM</v>
       </c>
       <c r="C54" t="str">
         <f>VLOOKUP(A54,FUND!A:D, 4, FALSE)</f>
-        <v>Guyana</v>
+        <v>Guatemala</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B55" t="str">
         <f>VLOOKUP(A55,FUND!A:C, 3, FALSE)</f>
-        <v>CHI</v>
+        <v>LAM</v>
       </c>
       <c r="C55" t="str">
         <f>VLOOKUP(A55,FUND!A:D, 4, FALSE)</f>
-        <v>Hong Kong</v>
+        <v>Guyana</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B56" t="str">
         <f>VLOOKUP(A56,FUND!A:C, 3, FALSE)</f>
-        <v>CAM</v>
+        <v>CHI</v>
       </c>
       <c r="C56" t="str">
         <f>VLOOKUP(A56,FUND!A:D, 4, FALSE)</f>
-        <v>Honduras</v>
+        <v>Hong Kong</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B57" t="str">
         <f>VLOOKUP(A57,FUND!A:C, 3, FALSE)</f>
-        <v>EEU</v>
+        <v>CAM</v>
       </c>
       <c r="C57" t="str">
         <f>VLOOKUP(A57,FUND!A:D, 4, FALSE)</f>
-        <v>Croatia</v>
+        <v>Honduras</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B58" t="str">
         <f>VLOOKUP(A58,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>EEU</v>
       </c>
       <c r="C58" t="str">
         <f>VLOOKUP(A58,FUND!A:D, 4, FALSE)</f>
-        <v>Haiti</v>
+        <v>Croatia</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B59" t="str">
         <f>VLOOKUP(A59,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>SIS</v>
       </c>
       <c r="C59" t="str">
         <f>VLOOKUP(A59,FUND!A:D, 4, FALSE)</f>
-        <v>Indonesia</v>
+        <v>Haiti</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B60" t="str">
         <f>VLOOKUP(A60,FUND!A:C, 3, FALSE)</f>
-        <v>SAS</v>
+        <v>SEA</v>
       </c>
       <c r="C60" t="str">
         <f>VLOOKUP(A60,FUND!A:D, 4, FALSE)</f>
-        <v>India</v>
+        <v>Indonesia</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B61" t="str">
         <f>VLOOKUP(A61,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SAS</v>
       </c>
       <c r="C61" t="str">
         <f>VLOOKUP(A61,FUND!A:D, 4, FALSE)</f>
-        <v>Ireland</v>
+        <v>India</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B62" t="str">
         <f>VLOOKUP(A62,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>WEU</v>
       </c>
       <c r="C62" t="str">
         <f>VLOOKUP(A62,FUND!A:D, 4, FALSE)</f>
-        <v>Iraq</v>
+        <v>Ireland</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B63" t="str">
         <f>VLOOKUP(A63,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>MDE</v>
       </c>
       <c r="C63" t="str">
         <f>VLOOKUP(A63,FUND!A:D, 4, FALSE)</f>
-        <v>Iceland</v>
+        <v>Iran, Islamic Republic of</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B64" t="str">
         <f>VLOOKUP(A64,FUND!A:C, 3, FALSE)</f>
@@ -13267,12 +13277,12 @@
       </c>
       <c r="C64" t="str">
         <f>VLOOKUP(A64,FUND!A:D, 4, FALSE)</f>
-        <v>Israel</v>
+        <v>Iraq</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B65" t="str">
         <f>VLOOKUP(A65,FUND!A:C, 3, FALSE)</f>
@@ -13280,337 +13290,337 @@
       </c>
       <c r="C65" t="str">
         <f>VLOOKUP(A65,FUND!A:D, 4, FALSE)</f>
-        <v>Italy</v>
+        <v>Iceland</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B66" t="str">
         <f>VLOOKUP(A66,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>MDE</v>
       </c>
       <c r="C66" t="str">
         <f>VLOOKUP(A66,FUND!A:D, 4, FALSE)</f>
-        <v>Jamaica</v>
+        <v>Israel</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B67" t="str">
         <f>VLOOKUP(A67,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>WEU</v>
       </c>
       <c r="C67" t="str">
         <f>VLOOKUP(A67,FUND!A:D, 4, FALSE)</f>
-        <v>Jordan</v>
+        <v>Italy</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B68" t="str">
         <f>VLOOKUP(A68,FUND!A:C, 3, FALSE)</f>
-        <v>JPK</v>
+        <v>SIS</v>
       </c>
       <c r="C68" t="str">
         <f>VLOOKUP(A68,FUND!A:D, 4, FALSE)</f>
-        <v>Japan</v>
+        <v>Jamaica</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B69" t="str">
         <f>VLOOKUP(A69,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>MDE</v>
       </c>
       <c r="C69" t="str">
         <f>VLOOKUP(A69,FUND!A:D, 4, FALSE)</f>
-        <v>Kenya</v>
+        <v>Jordan</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B70" t="str">
         <f>VLOOKUP(A70,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>JPK</v>
       </c>
       <c r="C70" t="str">
         <f>VLOOKUP(A70,FUND!A:D, 4, FALSE)</f>
-        <v>Cambodia</v>
+        <v>Japan</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B71" t="str">
         <f>VLOOKUP(A71,FUND!A:C, 3, FALSE)</f>
-        <v>JPK</v>
+        <v>SSA</v>
       </c>
       <c r="C71" t="str">
         <f>VLOOKUP(A71,FUND!A:D, 4, FALSE)</f>
-        <v>Korea, Republic of</v>
+        <v>Kenya</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B72" t="str">
         <f>VLOOKUP(A72,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>SEA</v>
       </c>
       <c r="C72" t="str">
         <f>VLOOKUP(A72,FUND!A:D, 4, FALSE)</f>
-        <v>Kuwait</v>
+        <v>Cambodia</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B73" t="str">
         <f>VLOOKUP(A73,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>JPK</v>
       </c>
       <c r="C73" t="str">
         <f>VLOOKUP(A73,FUND!A:D, 4, FALSE)</f>
-        <v>Lebanon</v>
+        <v>Korea, Republic of</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B74" t="str">
         <f>VLOOKUP(A74,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>MDE</v>
       </c>
       <c r="C74" t="str">
         <f>VLOOKUP(A74,FUND!A:D, 4, FALSE)</f>
-        <v>Liberia</v>
+        <v>Kuwait</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B75" t="str">
         <f>VLOOKUP(A75,FUND!A:C, 3, FALSE)</f>
-        <v>MAF</v>
+        <v>MDE</v>
       </c>
       <c r="C75" t="str">
         <f>VLOOKUP(A75,FUND!A:D, 4, FALSE)</f>
-        <v>Libya</v>
+        <v>Lebanon</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B76" t="str">
         <f>VLOOKUP(A76,FUND!A:C, 3, FALSE)</f>
-        <v>SAS</v>
+        <v>SSA</v>
       </c>
       <c r="C76" t="str">
         <f>VLOOKUP(A76,FUND!A:D, 4, FALSE)</f>
-        <v>Sri Lanka</v>
+        <v>Liberia</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B77" t="str">
         <f>VLOOKUP(A77,FUND!A:C, 3, FALSE)</f>
-        <v>FSU</v>
+        <v>MAF</v>
       </c>
       <c r="C77" t="str">
         <f>VLOOKUP(A77,FUND!A:D, 4, FALSE)</f>
-        <v>Lithuania</v>
+        <v>Libya</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B78" t="str">
         <f>VLOOKUP(A78,FUND!A:C, 3, FALSE)</f>
-        <v>FSU</v>
+        <v>SIS</v>
       </c>
       <c r="C78" t="str">
         <f>VLOOKUP(A78,FUND!A:D, 4, FALSE)</f>
-        <v>Latvia</v>
+        <v>Saint Lucia</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B79" t="str">
         <f>VLOOKUP(A79,FUND!A:C, 3, FALSE)</f>
-        <v>CHI</v>
+        <v>SAS</v>
       </c>
       <c r="C79" t="str">
         <f>VLOOKUP(A79,FUND!A:D, 4, FALSE)</f>
-        <v>Macao</v>
+        <v>Sri Lanka</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B80" t="str">
         <f>VLOOKUP(A80,FUND!A:C, 3, FALSE)</f>
-        <v>MAF</v>
+        <v>FSU</v>
       </c>
       <c r="C80" t="str">
         <f>VLOOKUP(A80,FUND!A:D, 4, FALSE)</f>
-        <v>Morocco</v>
+        <v>Lithuania</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B81" t="str">
         <f>VLOOKUP(A81,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>FSU</v>
       </c>
       <c r="C81" t="str">
         <f>VLOOKUP(A81,FUND!A:D, 4, FALSE)</f>
-        <v>Madagascar</v>
+        <v>Latvia</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B82" t="str">
         <f>VLOOKUP(A82,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>CHI</v>
       </c>
       <c r="C82" t="str">
         <f>VLOOKUP(A82,FUND!A:D, 4, FALSE)</f>
-        <v>Maldives</v>
+        <v>Macao</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B83" t="str">
         <f>VLOOKUP(A83,FUND!A:C, 3, FALSE)</f>
-        <v>CAM</v>
+        <v>MAF</v>
       </c>
       <c r="C83" t="str">
         <f>VLOOKUP(A83,FUND!A:D, 4, FALSE)</f>
-        <v>Mexico</v>
+        <v>Morocco</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B84" t="str">
         <f>VLOOKUP(A84,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SSA</v>
       </c>
       <c r="C84" t="str">
         <f>VLOOKUP(A84,FUND!A:D, 4, FALSE)</f>
-        <v>Malta</v>
+        <v>Madagascar</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B85" t="str">
         <f>VLOOKUP(A85,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>SIS</v>
       </c>
       <c r="C85" t="str">
         <f>VLOOKUP(A85,FUND!A:D, 4, FALSE)</f>
-        <v>Burma</v>
+        <v>Maldives</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B86" t="str">
         <f>VLOOKUP(A86,FUND!A:C, 3, FALSE)</f>
-        <v>EEU</v>
+        <v>CAM</v>
       </c>
       <c r="C86" t="str">
         <f>VLOOKUP(A86,FUND!A:D, 4, FALSE)</f>
-        <v>Montenegro</v>
+        <v>Mexico</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B87" t="str">
         <f>VLOOKUP(A87,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>WEU</v>
       </c>
       <c r="C87" t="str">
         <f>VLOOKUP(A87,FUND!A:D, 4, FALSE)</f>
-        <v>Mozambique</v>
+        <v>Malta</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B88" t="str">
         <f>VLOOKUP(A88,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>SEA</v>
       </c>
       <c r="C88" t="str">
         <f>VLOOKUP(A88,FUND!A:D, 4, FALSE)</f>
-        <v>Mauritania</v>
+        <v>Burma</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B89" t="str">
         <f>VLOOKUP(A89,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>EEU</v>
       </c>
       <c r="C89" t="str">
         <f>VLOOKUP(A89,FUND!A:D, 4, FALSE)</f>
-        <v>Mauritius</v>
+        <v>Montenegro</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B90" t="str">
         <f>VLOOKUP(A90,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>SSA</v>
       </c>
       <c r="C90" t="str">
         <f>VLOOKUP(A90,FUND!A:D, 4, FALSE)</f>
-        <v>Malaysia</v>
+        <v>Mozambique</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B91" t="str">
         <f>VLOOKUP(A91,FUND!A:C, 3, FALSE)</f>
@@ -13618,12 +13628,12 @@
       </c>
       <c r="C91" t="str">
         <f>VLOOKUP(A91,FUND!A:D, 4, FALSE)</f>
-        <v>Namibia</v>
+        <v>Mauritania</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B92" t="str">
         <f>VLOOKUP(A92,FUND!A:C, 3, FALSE)</f>
@@ -13631,311 +13641,311 @@
       </c>
       <c r="C92" t="str">
         <f>VLOOKUP(A92,FUND!A:D, 4, FALSE)</f>
-        <v>New Caledonia</v>
+        <v>Mauritius</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B93" t="str">
         <f>VLOOKUP(A93,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>SEA</v>
       </c>
       <c r="C93" t="str">
         <f>VLOOKUP(A93,FUND!A:D, 4, FALSE)</f>
-        <v>Nigeria</v>
+        <v>Malaysia</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B94" t="str">
         <f>VLOOKUP(A94,FUND!A:C, 3, FALSE)</f>
-        <v>CAM</v>
+        <v>SSA</v>
       </c>
       <c r="C94" t="str">
         <f>VLOOKUP(A94,FUND!A:D, 4, FALSE)</f>
-        <v>Nicaragua</v>
+        <v>Namibia</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B95" t="str">
         <f>VLOOKUP(A95,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SIS</v>
       </c>
       <c r="C95" t="str">
         <f>VLOOKUP(A95,FUND!A:D, 4, FALSE)</f>
-        <v>Netherlands</v>
+        <v>New Caledonia</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B96" t="str">
         <f>VLOOKUP(A96,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SSA</v>
       </c>
       <c r="C96" t="str">
         <f>VLOOKUP(A96,FUND!A:D, 4, FALSE)</f>
-        <v>Norway</v>
+        <v>Nigeria</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B97" t="str">
         <f>VLOOKUP(A97,FUND!A:C, 3, FALSE)</f>
-        <v>ANZ</v>
+        <v>CAM</v>
       </c>
       <c r="C97" t="str">
         <f>VLOOKUP(A97,FUND!A:D, 4, FALSE)</f>
-        <v>New Zealand</v>
+        <v>Nicaragua</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B98" t="str">
         <f>VLOOKUP(A98,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>WEU</v>
       </c>
       <c r="C98" t="str">
         <f>VLOOKUP(A98,FUND!A:D, 4, FALSE)</f>
-        <v>Oman</v>
+        <v>Netherlands</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B99" t="str">
         <f>VLOOKUP(A99,FUND!A:C, 3, FALSE)</f>
-        <v>SAS</v>
+        <v>WEU</v>
       </c>
       <c r="C99" t="str">
         <f>VLOOKUP(A99,FUND!A:D, 4, FALSE)</f>
-        <v>Pakistan</v>
+        <v>Norway</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B100" t="str">
         <f>VLOOKUP(A100,FUND!A:C, 3, FALSE)</f>
-        <v>CAM</v>
+        <v>ANZ</v>
       </c>
       <c r="C100" t="str">
         <f>VLOOKUP(A100,FUND!A:D, 4, FALSE)</f>
-        <v>Panama</v>
+        <v>New Zealand</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B101" t="str">
         <f>VLOOKUP(A101,FUND!A:C, 3, FALSE)</f>
-        <v>LAM</v>
+        <v>MDE</v>
       </c>
       <c r="C101" t="str">
         <f>VLOOKUP(A101,FUND!A:D, 4, FALSE)</f>
-        <v>Peru</v>
+        <v>Oman</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B102" t="str">
         <f>VLOOKUP(A102,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>SAS</v>
       </c>
       <c r="C102" t="str">
         <f>VLOOKUP(A102,FUND!A:D, 4, FALSE)</f>
-        <v>Philippines</v>
+        <v>Pakistan</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B103" t="str">
         <f>VLOOKUP(A103,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>CAM</v>
       </c>
       <c r="C103" t="str">
         <f>VLOOKUP(A103,FUND!A:D, 4, FALSE)</f>
-        <v>Papua New Guinea</v>
+        <v>Panama</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B104" t="str">
         <f>VLOOKUP(A104,FUND!A:C, 3, FALSE)</f>
-        <v>EEU</v>
+        <v>LAM</v>
       </c>
       <c r="C104" t="str">
         <f>VLOOKUP(A104,FUND!A:D, 4, FALSE)</f>
-        <v>Poland</v>
+        <v>Peru</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B105" t="str">
         <f>VLOOKUP(A105,FUND!A:C, 3, FALSE)</f>
-        <v>CAM</v>
+        <v>SEA</v>
       </c>
       <c r="C105" t="str">
         <f>VLOOKUP(A105,FUND!A:D, 4, FALSE)</f>
-        <v>Puerto Rico</v>
+        <v>Philippines</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B106" t="str">
         <f>VLOOKUP(A106,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SEA</v>
       </c>
       <c r="C106" t="str">
         <f>VLOOKUP(A106,FUND!A:D, 4, FALSE)</f>
-        <v>Portugal</v>
+        <v>Papua New Guinea</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B107" t="str">
         <f>VLOOKUP(A107,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>EEU</v>
       </c>
       <c r="C107" t="str">
         <f>VLOOKUP(A107,FUND!A:D, 4, FALSE)</f>
-        <v>French Polynesia</v>
+        <v>Poland</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B108" t="str">
         <f>VLOOKUP(A108,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>CAM</v>
       </c>
       <c r="C108" t="str">
         <f>VLOOKUP(A108,FUND!A:D, 4, FALSE)</f>
-        <v>Qatar</v>
+        <v>Puerto Rico</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B109" t="str">
         <f>VLOOKUP(A109,FUND!A:C, 3, FALSE)</f>
-        <v>EEU</v>
+        <v>WEU</v>
       </c>
       <c r="C109" t="str">
         <f>VLOOKUP(A109,FUND!A:D, 4, FALSE)</f>
-        <v>Romania</v>
+        <v>Portugal</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B110" t="str">
         <f>VLOOKUP(A110,FUND!A:C, 3, FALSE)</f>
-        <v>FSU</v>
+        <v>MDE</v>
       </c>
       <c r="C110" t="str">
         <f>VLOOKUP(A110,FUND!A:D, 4, FALSE)</f>
-        <v>Russia</v>
+        <v>Palestinian Territory, Occupied</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="B111" t="str">
         <f>VLOOKUP(A111,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>SIS</v>
       </c>
       <c r="C111" t="str">
         <f>VLOOKUP(A111,FUND!A:D, 4, FALSE)</f>
-        <v>Saudi Arabia</v>
+        <v>French Polynesia</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="B112" t="str">
         <f>VLOOKUP(A112,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>MDE</v>
       </c>
       <c r="C112" t="str">
         <f>VLOOKUP(A112,FUND!A:D, 4, FALSE)</f>
-        <v>Sudan</v>
+        <v>Qatar</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B113" t="str">
         <f>VLOOKUP(A113,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>EEU</v>
       </c>
       <c r="C113" t="str">
         <f>VLOOKUP(A113,FUND!A:D, 4, FALSE)</f>
-        <v>Senegal</v>
+        <v>Romania</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B114" t="str">
         <f>VLOOKUP(A114,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>FSU</v>
       </c>
       <c r="C114" t="str">
         <f>VLOOKUP(A114,FUND!A:D, 4, FALSE)</f>
-        <v>Singapore</v>
+        <v>Russia</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B115" t="str">
         <f>VLOOKUP(A115,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>MDE</v>
       </c>
       <c r="C115" t="str">
         <f>VLOOKUP(A115,FUND!A:D, 4, FALSE)</f>
-        <v>Solomon Islands</v>
+        <v>Saudi Arabia</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B116" t="str">
         <f>VLOOKUP(A116,FUND!A:C, 3, FALSE)</f>
@@ -13943,38 +13953,38 @@
       </c>
       <c r="C116" t="str">
         <f>VLOOKUP(A116,FUND!A:D, 4, FALSE)</f>
-        <v>Sierra Leone</v>
+        <v>Sudan</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B117" t="str">
         <f>VLOOKUP(A117,FUND!A:C, 3, FALSE)</f>
-        <v>CAM</v>
+        <v>SSA</v>
       </c>
       <c r="C117" t="str">
         <f>VLOOKUP(A117,FUND!A:D, 4, FALSE)</f>
-        <v>El Salvador</v>
+        <v>Senegal</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B118" t="str">
         <f>VLOOKUP(A118,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>SEA</v>
       </c>
       <c r="C118" t="str">
         <f>VLOOKUP(A118,FUND!A:D, 4, FALSE)</f>
-        <v>Somalia</v>
+        <v>Singapore</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B119" t="str">
         <f>VLOOKUP(A119,FUND!A:C, 3, FALSE)</f>
@@ -13982,272 +13992,272 @@
       </c>
       <c r="C119" t="str">
         <f>VLOOKUP(A119,FUND!A:D, 4, FALSE)</f>
-        <v>Sao Tome and Principe</v>
+        <v>Solomon Islands</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="B120" t="str">
         <f>VLOOKUP(A120,FUND!A:C, 3, FALSE)</f>
-        <v>LAM</v>
+        <v>SSA</v>
       </c>
       <c r="C120" t="str">
         <f>VLOOKUP(A120,FUND!A:D, 4, FALSE)</f>
-        <v>Suriname</v>
+        <v>Sierra Leone</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B121" t="str">
         <f>VLOOKUP(A121,FUND!A:C, 3, FALSE)</f>
-        <v>EEU</v>
+        <v>CAM</v>
       </c>
       <c r="C121" t="str">
         <f>VLOOKUP(A121,FUND!A:D, 4, FALSE)</f>
-        <v>Slovenia</v>
+        <v>El Salvador</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B122" t="str">
         <f>VLOOKUP(A122,FUND!A:C, 3, FALSE)</f>
-        <v>WEU</v>
+        <v>SSA</v>
       </c>
       <c r="C122" t="str">
         <f>VLOOKUP(A122,FUND!A:D, 4, FALSE)</f>
-        <v>Sweden</v>
+        <v>Somalia</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B123" t="str">
         <f>VLOOKUP(A123,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>SIS</v>
       </c>
       <c r="C123" t="str">
         <f>VLOOKUP(A123,FUND!A:D, 4, FALSE)</f>
-        <v>Syrian Arab Republic</v>
+        <v>Sao Tome and Principe</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="B124" t="str">
         <f>VLOOKUP(A124,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>LAM</v>
       </c>
       <c r="C124" t="str">
         <f>VLOOKUP(A124,FUND!A:D, 4, FALSE)</f>
-        <v>Togo</v>
+        <v>Suriname</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="B125" t="str">
         <f>VLOOKUP(A125,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>EEU</v>
       </c>
       <c r="C125" t="str">
         <f>VLOOKUP(A125,FUND!A:D, 4, FALSE)</f>
-        <v>Thailand</v>
+        <v>Slovenia</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B126" t="str">
         <f>VLOOKUP(A126,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>WEU</v>
       </c>
       <c r="C126" t="str">
         <f>VLOOKUP(A126,FUND!A:D, 4, FALSE)</f>
-        <v>Timor-Leste</v>
+        <v>Sweden</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B127" t="str">
         <f>VLOOKUP(A127,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>MDE</v>
       </c>
       <c r="C127" t="str">
         <f>VLOOKUP(A127,FUND!A:D, 4, FALSE)</f>
-        <v>Tonga</v>
+        <v>Syrian Arab Republic</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B128" t="str">
         <f>VLOOKUP(A128,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>SSA</v>
       </c>
       <c r="C128" t="str">
         <f>VLOOKUP(A128,FUND!A:D, 4, FALSE)</f>
-        <v>Trinidad and Tobago</v>
+        <v>Togo</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="B129" t="str">
         <f>VLOOKUP(A129,FUND!A:C, 3, FALSE)</f>
-        <v>MAF</v>
+        <v>SEA</v>
       </c>
       <c r="C129" t="str">
         <f>VLOOKUP(A129,FUND!A:D, 4, FALSE)</f>
-        <v>Tunisia</v>
+        <v>Thailand</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B130" t="str">
         <f>VLOOKUP(A130,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>SEA</v>
       </c>
       <c r="C130" t="str">
         <f>VLOOKUP(A130,FUND!A:D, 4, FALSE)</f>
-        <v>Turkey</v>
+        <v>Timor-Leste</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B131" t="str">
         <f>VLOOKUP(A131,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>SIS</v>
       </c>
       <c r="C131" t="str">
         <f>VLOOKUP(A131,FUND!A:D, 4, FALSE)</f>
-        <v>Taiwan</v>
+        <v>Tonga</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B132" t="str">
         <f>VLOOKUP(A132,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>SIS</v>
       </c>
       <c r="C132" t="str">
         <f>VLOOKUP(A132,FUND!A:D, 4, FALSE)</f>
-        <v>Tanzania, United Republic of</v>
+        <v>Trinidad and Tobago</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B133" t="str">
         <f>VLOOKUP(A133,FUND!A:C, 3, FALSE)</f>
-        <v>FSU</v>
+        <v>MAF</v>
       </c>
       <c r="C133" t="str">
         <f>VLOOKUP(A133,FUND!A:D, 4, FALSE)</f>
-        <v>Ukraine</v>
+        <v>Tunisia</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B134" t="str">
         <f>VLOOKUP(A134,FUND!A:C, 3, FALSE)</f>
-        <v>LAM</v>
+        <v>MDE</v>
       </c>
       <c r="C134" t="str">
         <f>VLOOKUP(A134,FUND!A:D, 4, FALSE)</f>
-        <v>Uruguay</v>
+        <v>Turkey</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>0</v>
+        <v>392</v>
       </c>
       <c r="B135" t="str">
         <f>VLOOKUP(A135,FUND!A:C, 3, FALSE)</f>
-        <v>USA</v>
+        <v>SEA</v>
       </c>
       <c r="C135" t="str">
         <f>VLOOKUP(A135,FUND!A:D, 4, FALSE)</f>
-        <v>United States</v>
+        <v>Taiwan</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="B136" t="str">
         <f>VLOOKUP(A136,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>SSA</v>
       </c>
       <c r="C136" t="str">
         <f>VLOOKUP(A136,FUND!A:D, 4, FALSE)</f>
-        <v>Saint Vincent &amp; the Grenadines</v>
+        <v>Tanzania, United Republic of</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B137" t="str">
         <f>VLOOKUP(A137,FUND!A:C, 3, FALSE)</f>
-        <v>LAM</v>
+        <v>FSU</v>
       </c>
       <c r="C137" t="str">
         <f>VLOOKUP(A137,FUND!A:D, 4, FALSE)</f>
-        <v>Venezuela</v>
+        <v>Ukraine</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="B138" t="str">
         <f>VLOOKUP(A138,FUND!A:C, 3, FALSE)</f>
-        <v>SEA</v>
+        <v>LAM</v>
       </c>
       <c r="C138" t="str">
         <f>VLOOKUP(A138,FUND!A:D, 4, FALSE)</f>
-        <v>Viet Nam</v>
+        <v>Uruguay</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>405</v>
+        <v>0</v>
       </c>
       <c r="B139" t="str">
         <f>VLOOKUP(A139,FUND!A:C, 3, FALSE)</f>
-        <v>SIS</v>
+        <v>USA</v>
       </c>
       <c r="C139" t="str">
         <f>VLOOKUP(A139,FUND!A:D, 4, FALSE)</f>
-        <v>Vanuatu</v>
+        <v>United States</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B140" t="str">
         <f>VLOOKUP(A140,FUND!A:C, 3, FALSE)</f>
@@ -14255,32 +14265,84 @@
       </c>
       <c r="C140" t="str">
         <f>VLOOKUP(A140,FUND!A:D, 4, FALSE)</f>
-        <v>Samoa</v>
+        <v>Saint Vincent &amp; the Grenadines</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="B141" t="str">
         <f>VLOOKUP(A141,FUND!A:C, 3, FALSE)</f>
-        <v>MDE</v>
+        <v>LAM</v>
       </c>
       <c r="C141" t="str">
         <f>VLOOKUP(A141,FUND!A:D, 4, FALSE)</f>
-        <v>Yemen</v>
+        <v>Venezuela</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B142" t="str">
         <f>VLOOKUP(A142,FUND!A:C, 3, FALSE)</f>
-        <v>SSA</v>
+        <v>SEA</v>
       </c>
       <c r="C142" t="str">
         <f>VLOOKUP(A142,FUND!A:D, 4, FALSE)</f>
+        <v>Viet Nam</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>405</v>
+      </c>
+      <c r="B143" t="str">
+        <f>VLOOKUP(A143,FUND!A:C, 3, FALSE)</f>
+        <v>SIS</v>
+      </c>
+      <c r="C143" t="str">
+        <f>VLOOKUP(A143,FUND!A:D, 4, FALSE)</f>
+        <v>Vanuatu</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>406</v>
+      </c>
+      <c r="B144" t="str">
+        <f>VLOOKUP(A144,FUND!A:C, 3, FALSE)</f>
+        <v>SIS</v>
+      </c>
+      <c r="C144" t="str">
+        <f>VLOOKUP(A144,FUND!A:D, 4, FALSE)</f>
+        <v>Samoa</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>407</v>
+      </c>
+      <c r="B145" t="str">
+        <f>VLOOKUP(A145,FUND!A:C, 3, FALSE)</f>
+        <v>MDE</v>
+      </c>
+      <c r="C145" t="str">
+        <f>VLOOKUP(A145,FUND!A:D, 4, FALSE)</f>
+        <v>Yemen</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>408</v>
+      </c>
+      <c r="B146" t="str">
+        <f>VLOOKUP(A146,FUND!A:C, 3, FALSE)</f>
+        <v>SSA</v>
+      </c>
+      <c r="C146" t="str">
+        <f>VLOOKUP(A146,FUND!A:D, 4, FALSE)</f>
         <v>South Africa</v>
       </c>
     </row>

</xml_diff>